<commit_message>
Still some bugs with the excel
</commit_message>
<xml_diff>
--- a/src/prueba.xlsx
+++ b/src/prueba.xlsx
@@ -7,7 +7,8 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Resultados" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Resultados" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -17,16 +18,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -37,7 +35,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -45,21 +43,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -425,7 +414,25 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C501"/>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A2:G501"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -433,23 +440,6 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Rockie</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Paperly</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Ganador</t>
-        </is>
-      </c>
-    </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
@@ -483,6 +473,16 @@
           <t>Paperly</t>
         </is>
       </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Rockie</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Paperly</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -499,6 +499,12 @@
         <is>
           <t>Paperly</t>
         </is>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="5">

</xml_diff>